<commit_message>
save up to 5 images URLs
</commit_message>
<xml_diff>
--- a/admin/linkdata.xlsx
+++ b/admin/linkdata.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\tweet2linkdata\admin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Tweet2LinkData\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="9855"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17235" windowHeight="9750"/>
   </bookViews>
   <sheets>
     <sheet name="LinkTable" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
   <si>
     <t>#LINK&lt;-- ファイルタイプの指定</t>
   </si>
@@ -519,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J99"/>
+  <dimension ref="A1:N99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -530,14 +530,14 @@
     <col min="3" max="3" width="40.875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.25" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="35" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="39.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="3"/>
+    <col min="6" max="10" width="21.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="35" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,13 +546,13 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -560,19 +560,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="7"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -592,19 +592,31 @@
         <v>18</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="M6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -635,8 +647,20 @@
       <c r="J7" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -656,19 +680,31 @@
         <v>12</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -679,8 +715,12 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -691,8 +731,12 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -703,8 +747,12 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -715,8 +763,12 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -727,8 +779,12 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -739,8 +795,12 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -751,8 +811,12 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -763,8 +827,12 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -775,8 +843,12 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -787,8 +859,12 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -799,8 +875,12 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -811,8 +891,12 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -823,8 +907,12 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -835,8 +923,12 @@
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -847,8 +939,12 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -859,8 +955,12 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -871,8 +971,12 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -883,8 +987,12 @@
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -895,8 +1003,12 @@
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -907,8 +1019,12 @@
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -919,8 +1035,12 @@
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -931,8 +1051,12 @@
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -943,8 +1067,12 @@
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -955,8 +1083,12 @@
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -967,8 +1099,12 @@
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -979,8 +1115,12 @@
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -991,8 +1131,12 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1003,8 +1147,12 @@
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -1015,8 +1163,12 @@
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1027,8 +1179,12 @@
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -1039,8 +1195,12 @@
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -1051,8 +1211,12 @@
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -1063,8 +1227,12 @@
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -1075,8 +1243,12 @@
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -1087,8 +1259,12 @@
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -1099,8 +1275,12 @@
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -1111,8 +1291,12 @@
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -1123,8 +1307,12 @@
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -1135,8 +1323,12 @@
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -1147,8 +1339,12 @@
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K48" s="6"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="6"/>
+      <c r="N48" s="6"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -1159,8 +1355,12 @@
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K49" s="6"/>
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -1171,8 +1371,12 @@
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K50" s="6"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="6"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -1183,8 +1387,12 @@
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -1195,8 +1403,12 @@
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" s="5"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -1207,8 +1419,12 @@
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6"/>
+      <c r="N53" s="6"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -1219,8 +1435,12 @@
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6"/>
+      <c r="N54" s="6"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" s="5"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -1231,8 +1451,12 @@
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K55" s="6"/>
+      <c r="L55" s="6"/>
+      <c r="M55" s="6"/>
+      <c r="N55" s="6"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" s="5"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -1243,8 +1467,12 @@
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K56" s="6"/>
+      <c r="L56" s="6"/>
+      <c r="M56" s="6"/>
+      <c r="N56" s="6"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" s="5"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -1255,8 +1483,12 @@
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K57" s="6"/>
+      <c r="L57" s="6"/>
+      <c r="M57" s="6"/>
+      <c r="N57" s="6"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" s="5"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -1267,8 +1499,12 @@
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K58" s="6"/>
+      <c r="L58" s="6"/>
+      <c r="M58" s="6"/>
+      <c r="N58" s="6"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" s="5"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -1279,8 +1515,12 @@
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
       <c r="J59" s="6"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K59" s="6"/>
+      <c r="L59" s="6"/>
+      <c r="M59" s="6"/>
+      <c r="N59" s="6"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60" s="5"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -1291,8 +1531,12 @@
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K60" s="6"/>
+      <c r="L60" s="6"/>
+      <c r="M60" s="6"/>
+      <c r="N60" s="6"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61" s="5"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -1303,8 +1547,12 @@
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="6"/>
+      <c r="N61" s="6"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62" s="5"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -1315,8 +1563,12 @@
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K62" s="6"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="6"/>
+      <c r="N62" s="6"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A63" s="5"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -1327,8 +1579,12 @@
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
       <c r="J63" s="6"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="6"/>
+      <c r="N63" s="6"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A64" s="5"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -1339,8 +1595,12 @@
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
       <c r="J64" s="6"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K64" s="6"/>
+      <c r="L64" s="6"/>
+      <c r="M64" s="6"/>
+      <c r="N64" s="6"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65" s="5"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -1351,8 +1611,12 @@
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
       <c r="J65" s="6"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
+      <c r="N65" s="6"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A66" s="5"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -1363,8 +1627,12 @@
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
       <c r="J66" s="6"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="6"/>
+      <c r="N66" s="6"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A67" s="5"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -1375,8 +1643,12 @@
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
       <c r="J67" s="6"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="6"/>
+      <c r="N67" s="6"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A68" s="5"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -1387,8 +1659,12 @@
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
       <c r="J68" s="6"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K68" s="6"/>
+      <c r="L68" s="6"/>
+      <c r="M68" s="6"/>
+      <c r="N68" s="6"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A69" s="5"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -1399,8 +1675,12 @@
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
       <c r="J69" s="6"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="6"/>
+      <c r="N69" s="6"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A70" s="5"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -1411,8 +1691,12 @@
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
       <c r="J70" s="6"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K70" s="6"/>
+      <c r="L70" s="6"/>
+      <c r="M70" s="6"/>
+      <c r="N70" s="6"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A71" s="5"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -1423,8 +1707,12 @@
       <c r="H71" s="6"/>
       <c r="I71" s="6"/>
       <c r="J71" s="6"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K71" s="6"/>
+      <c r="L71" s="6"/>
+      <c r="M71" s="6"/>
+      <c r="N71" s="6"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A72" s="5"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -1435,8 +1723,12 @@
       <c r="H72" s="6"/>
       <c r="I72" s="6"/>
       <c r="J72" s="6"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K72" s="6"/>
+      <c r="L72" s="6"/>
+      <c r="M72" s="6"/>
+      <c r="N72" s="6"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A73" s="5"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -1447,8 +1739,12 @@
       <c r="H73" s="6"/>
       <c r="I73" s="6"/>
       <c r="J73" s="6"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K73" s="6"/>
+      <c r="L73" s="6"/>
+      <c r="M73" s="6"/>
+      <c r="N73" s="6"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A74" s="5"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -1459,8 +1755,12 @@
       <c r="H74" s="6"/>
       <c r="I74" s="6"/>
       <c r="J74" s="6"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K74" s="6"/>
+      <c r="L74" s="6"/>
+      <c r="M74" s="6"/>
+      <c r="N74" s="6"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A75" s="5"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -1471,8 +1771,12 @@
       <c r="H75" s="6"/>
       <c r="I75" s="6"/>
       <c r="J75" s="6"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K75" s="6"/>
+      <c r="L75" s="6"/>
+      <c r="M75" s="6"/>
+      <c r="N75" s="6"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A76" s="5"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -1483,8 +1787,12 @@
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
       <c r="J76" s="6"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K76" s="6"/>
+      <c r="L76" s="6"/>
+      <c r="M76" s="6"/>
+      <c r="N76" s="6"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A77" s="5"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -1495,8 +1803,12 @@
       <c r="H77" s="6"/>
       <c r="I77" s="6"/>
       <c r="J77" s="6"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+      <c r="M77" s="6"/>
+      <c r="N77" s="6"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A78" s="5"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -1507,8 +1819,12 @@
       <c r="H78" s="6"/>
       <c r="I78" s="6"/>
       <c r="J78" s="6"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K78" s="6"/>
+      <c r="L78" s="6"/>
+      <c r="M78" s="6"/>
+      <c r="N78" s="6"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A79" s="5"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
@@ -1519,8 +1835,12 @@
       <c r="H79" s="6"/>
       <c r="I79" s="6"/>
       <c r="J79" s="6"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K79" s="6"/>
+      <c r="L79" s="6"/>
+      <c r="M79" s="6"/>
+      <c r="N79" s="6"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A80" s="5"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
@@ -1531,8 +1851,12 @@
       <c r="H80" s="6"/>
       <c r="I80" s="6"/>
       <c r="J80" s="6"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K80" s="6"/>
+      <c r="L80" s="6"/>
+      <c r="M80" s="6"/>
+      <c r="N80" s="6"/>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A81" s="5"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
@@ -1543,8 +1867,12 @@
       <c r="H81" s="6"/>
       <c r="I81" s="6"/>
       <c r="J81" s="6"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="6"/>
+      <c r="N81" s="6"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A82" s="5"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -1555,8 +1883,12 @@
       <c r="H82" s="6"/>
       <c r="I82" s="6"/>
       <c r="J82" s="6"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="6"/>
+      <c r="N82" s="6"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A83" s="5"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -1567,8 +1899,12 @@
       <c r="H83" s="6"/>
       <c r="I83" s="6"/>
       <c r="J83" s="6"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K83" s="6"/>
+      <c r="L83" s="6"/>
+      <c r="M83" s="6"/>
+      <c r="N83" s="6"/>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A84" s="5"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -1579,8 +1915,12 @@
       <c r="H84" s="6"/>
       <c r="I84" s="6"/>
       <c r="J84" s="6"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K84" s="6"/>
+      <c r="L84" s="6"/>
+      <c r="M84" s="6"/>
+      <c r="N84" s="6"/>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A85" s="5"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -1591,8 +1931,12 @@
       <c r="H85" s="6"/>
       <c r="I85" s="6"/>
       <c r="J85" s="6"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K85" s="6"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="6"/>
+      <c r="N85" s="6"/>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A86" s="5"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -1603,8 +1947,12 @@
       <c r="H86" s="6"/>
       <c r="I86" s="6"/>
       <c r="J86" s="6"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K86" s="6"/>
+      <c r="L86" s="6"/>
+      <c r="M86" s="6"/>
+      <c r="N86" s="6"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A87" s="5"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -1615,8 +1963,12 @@
       <c r="H87" s="6"/>
       <c r="I87" s="6"/>
       <c r="J87" s="6"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K87" s="6"/>
+      <c r="L87" s="6"/>
+      <c r="M87" s="6"/>
+      <c r="N87" s="6"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A88" s="5"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -1627,8 +1979,12 @@
       <c r="H88" s="6"/>
       <c r="I88" s="6"/>
       <c r="J88" s="6"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K88" s="6"/>
+      <c r="L88" s="6"/>
+      <c r="M88" s="6"/>
+      <c r="N88" s="6"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A89" s="5"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -1639,8 +1995,12 @@
       <c r="H89" s="6"/>
       <c r="I89" s="6"/>
       <c r="J89" s="6"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K89" s="6"/>
+      <c r="L89" s="6"/>
+      <c r="M89" s="6"/>
+      <c r="N89" s="6"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A90" s="5"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -1651,8 +2011,12 @@
       <c r="H90" s="6"/>
       <c r="I90" s="6"/>
       <c r="J90" s="6"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K90" s="6"/>
+      <c r="L90" s="6"/>
+      <c r="M90" s="6"/>
+      <c r="N90" s="6"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A91" s="5"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -1663,8 +2027,12 @@
       <c r="H91" s="6"/>
       <c r="I91" s="6"/>
       <c r="J91" s="6"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K91" s="6"/>
+      <c r="L91" s="6"/>
+      <c r="M91" s="6"/>
+      <c r="N91" s="6"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A92" s="5"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -1675,8 +2043,12 @@
       <c r="H92" s="6"/>
       <c r="I92" s="6"/>
       <c r="J92" s="6"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K92" s="6"/>
+      <c r="L92" s="6"/>
+      <c r="M92" s="6"/>
+      <c r="N92" s="6"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A93" s="5"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -1687,8 +2059,12 @@
       <c r="H93" s="6"/>
       <c r="I93" s="6"/>
       <c r="J93" s="6"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K93" s="6"/>
+      <c r="L93" s="6"/>
+      <c r="M93" s="6"/>
+      <c r="N93" s="6"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A94" s="5"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -1699,8 +2075,12 @@
       <c r="H94" s="6"/>
       <c r="I94" s="6"/>
       <c r="J94" s="6"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K94" s="6"/>
+      <c r="L94" s="6"/>
+      <c r="M94" s="6"/>
+      <c r="N94" s="6"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A95" s="5"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -1711,8 +2091,12 @@
       <c r="H95" s="6"/>
       <c r="I95" s="6"/>
       <c r="J95" s="6"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K95" s="6"/>
+      <c r="L95" s="6"/>
+      <c r="M95" s="6"/>
+      <c r="N95" s="6"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A96" s="5"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -1723,8 +2107,12 @@
       <c r="H96" s="6"/>
       <c r="I96" s="6"/>
       <c r="J96" s="6"/>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K96" s="6"/>
+      <c r="L96" s="6"/>
+      <c r="M96" s="6"/>
+      <c r="N96" s="6"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A97" s="5"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
@@ -1735,8 +2123,12 @@
       <c r="H97" s="6"/>
       <c r="I97" s="6"/>
       <c r="J97" s="6"/>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K97" s="6"/>
+      <c r="L97" s="6"/>
+      <c r="M97" s="6"/>
+      <c r="N97" s="6"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A98" s="5"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -1747,8 +2139,12 @@
       <c r="H98" s="6"/>
       <c r="I98" s="6"/>
       <c r="J98" s="6"/>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K98" s="6"/>
+      <c r="L98" s="6"/>
+      <c r="M98" s="6"/>
+      <c r="N98" s="6"/>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A99" s="5"/>
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
@@ -1759,6 +2155,10 @@
       <c r="H99" s="6"/>
       <c r="I99" s="6"/>
       <c r="J99" s="6"/>
+      <c r="K99" s="6"/>
+      <c r="L99" s="6"/>
+      <c r="M99" s="6"/>
+      <c r="N99" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>